<commit_message>
finished q191 and q237 in mocked_assessment/trial1
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python\leetcode.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CB97F4-BB4B-44AE-9E93-2DB9B7A6F877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF15A967-7E52-4FFA-8483-22F6B6AE7D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>Problem</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>Permutation in String</t>
+  </si>
+  <si>
+    <t>Delete Node in a Linked List</t>
+  </si>
+  <si>
+    <t>Number of 1 Bits</t>
   </si>
 </sst>
 </file>
@@ -313,7 +319,49 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -674,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,16 +754,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>22</v>
+        <v>441</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="12">
-        <v>44537.487768402774</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
+        <v>44505</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
@@ -723,10 +768,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>441</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>33</v>
+        <v>1489</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="C3" s="12">
         <v>44505</v>
@@ -737,13 +782,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1489</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>39</v>
+        <v>121</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="C4" s="12">
-        <v>44505</v>
+        <v>44510</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>4</v>
@@ -751,13 +799,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="12">
-        <v>44510</v>
+        <v>44511</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -768,64 +816,61 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>122</v>
+        <v>35</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6" s="12">
-        <v>44511</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
+        <v>44516</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>35</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>23</v>
+        <v>278</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="C7" s="12">
         <v>44516</v>
       </c>
       <c r="I7" s="10">
         <f ca="1">NOW()</f>
-        <v>44537.487861226851</v>
+        <v>44537.698034027781</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>278</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>29</v>
+        <v>309</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="C8" s="12">
         <v>44516</v>
       </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>309</v>
+        <v>704</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C9" s="12">
         <v>44516</v>
       </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>704</v>
+        <v>714</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="12">
         <v>44516</v>
@@ -833,21 +878,21 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>714</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>36</v>
+        <v>189</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="C11" s="12">
-        <v>44516</v>
+        <v>44517</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>189</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>28</v>
+        <v>977</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="C12" s="12">
         <v>44517</v>
@@ -855,38 +900,41 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>977</v>
+        <v>283</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C13" s="12">
-        <v>44517</v>
+        <v>44518</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>283</v>
+        <v>167</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C14" s="12">
         <v>44518</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>167</v>
+        <v>344</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C15" s="12">
-        <v>44518</v>
+        <v>44519</v>
       </c>
       <c r="D15" t="s">
         <v>24</v>
@@ -894,93 +942,90 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>344</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>32</v>
+        <v>557</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C16" s="12">
         <v>44519</v>
       </c>
       <c r="D16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="12">
+        <v>44522</v>
+      </c>
+      <c r="D17" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>557</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="12">
-        <v>44519</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C18" s="12">
-        <v>44522</v>
+        <v>44524</v>
       </c>
       <c r="D18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="11">
+        <v>44524</v>
+      </c>
+      <c r="D19" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="12">
-        <v>44524</v>
-      </c>
-      <c r="D19" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C20" s="11">
-        <v>44524</v>
+        <v>44529</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="7" t="s">
-        <v>7</v>
+      <c r="A21">
+        <v>328</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="C21" s="11">
-        <v>44529</v>
+        <v>44530</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>328</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>13</v>
+      <c r="B22" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C22" s="11">
         <v>44530</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C23" s="11">
         <v>44530</v>
@@ -990,8 +1035,11 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="9" t="s">
-        <v>9</v>
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="C24" s="11">
         <v>44530</v>
@@ -1002,119 +1050,173 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>19</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>8</v>
+        <v>234</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="C25" s="11">
-        <v>44530</v>
+        <v>44531</v>
       </c>
       <c r="D25" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>234</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>15</v>
+      <c r="B26" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C26" s="11">
-        <v>44531</v>
+        <v>44532</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C27" s="11">
         <v>44532</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2</v>
+      </c>
       <c r="B28" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C28" s="11">
-        <v>44532</v>
+        <v>44533.546204976854</v>
       </c>
       <c r="D28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="12">
+        <v>44536.512189930552</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="12">
+        <v>44536.543766666669</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>876</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="12">
+        <v>44536.639974189813</v>
+      </c>
+      <c r="D31" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>2</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="11">
-        <v>44533.546204976854</v>
-      </c>
-      <c r="D29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="12">
-        <v>44536.512189930552</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="12">
-        <v>44536.543766666669</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>876</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>42</v>
+        <v>567</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="C32" s="12">
-        <v>44536.639974189813</v>
+        <v>44536.742515162034</v>
       </c>
       <c r="D32" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>567</v>
+        <v>3</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C33" s="12">
-        <v>44536.742515162034</v>
+        <v>44537.487768402774</v>
       </c>
       <c r="D33" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>237</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="12">
+        <v>44537.696392245372</v>
+      </c>
+      <c r="D34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>191</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="12">
+        <v>44537.696392245372</v>
+      </c>
+      <c r="D35" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D33">
+      <sortCondition ref="C1"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C12">
     <sortCondition descending="1" ref="C2:C12"/>
     <sortCondition descending="1" ref="B2:B12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D30 D34:D101">
+  <conditionalFormatting sqref="D2:D30 D36:D101">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1125,7 +1227,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D33">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1136,7 +1238,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D34">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1147,7 +1249,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
+  <conditionalFormatting sqref="D35">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>

</xml_diff>

<commit_message>
finish q5, q973 in mocked_assessment/trial2
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python\leetcode.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF15A967-7E52-4FFA-8483-22F6B6AE7D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573E02C1-344B-45D3-8489-90CEF22693E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58815" yWindow="1770" windowWidth="12960" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t>Problem</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t>Number of 1 Bits</t>
+  </si>
+  <si>
+    <t>K Closest Points to Origin</t>
+  </si>
+  <si>
+    <t>Longest Palindromic Substring</t>
   </si>
 </sst>
 </file>
@@ -319,7 +325,49 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -722,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -837,7 +885,7 @@
       </c>
       <c r="I7" s="10">
         <f ca="1">NOW()</f>
-        <v>44537.698034027781</v>
+        <v>44537.760845486111</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1182,6 +1230,34 @@
       </c>
       <c r="D35" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>973</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="12">
+        <v>44537.758970023147</v>
+      </c>
+      <c r="D36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="12">
+        <v>44537.759664351855</v>
+      </c>
+      <c r="D37" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1194,7 +1270,29 @@
     <sortCondition descending="1" ref="C2:C12"/>
     <sortCondition descending="1" ref="B2:B12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D30 D36:D101">
+  <conditionalFormatting sqref="D2:D30 D38:D101">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1205,7 +1303,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D33">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1216,7 +1314,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D34">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1227,7 +1325,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
+  <conditionalFormatting sqref="D35">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1238,7 +1336,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
+  <conditionalFormatting sqref="D36">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1249,7 +1347,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
+  <conditionalFormatting sqref="D37">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>

</xml_diff>

<commit_message>
q695 and fix qnnn/test_.py to fix pytest bug
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python\leetcode.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573E02C1-344B-45D3-8489-90CEF22693E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA0408E-A5B5-425B-B9CA-C9A04E645EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58815" yWindow="1770" windowWidth="12960" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
   <si>
     <t>Problem</t>
   </si>
@@ -227,6 +227,15 @@
   </si>
   <si>
     <t>Longest Palindromic Substring</t>
+  </si>
+  <si>
+    <t>Minimum Number of Taps to Open to Water a Garden</t>
+  </si>
+  <si>
+    <t>Flood Fill</t>
+  </si>
+  <si>
+    <t>Max Area of Island</t>
   </si>
 </sst>
 </file>
@@ -325,7 +334,49 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -770,16 +821,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="40.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="76.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -885,7 +936,7 @@
       </c>
       <c r="I7" s="10">
         <f ca="1">NOW()</f>
-        <v>44537.760845486111</v>
+        <v>44545.580656018516</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1257,6 +1308,48 @@
         <v>44537.759664351855</v>
       </c>
       <c r="D37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>1326</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="12">
+        <v>44544.671527777777</v>
+      </c>
+      <c r="D38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>733</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="12">
+        <v>44545.451388888891</v>
+      </c>
+      <c r="D39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>695</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="12">
+        <v>44545.58037152778</v>
+      </c>
+      <c r="D40" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1270,7 +1363,29 @@
     <sortCondition descending="1" ref="C2:C12"/>
     <sortCondition descending="1" ref="B2:B12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D30 D38:D101">
+  <conditionalFormatting sqref="D2:D30 D38 D41:D101">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
     <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1281,7 +1396,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D33">
     <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1292,7 +1407,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D34">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1303,7 +1418,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
+  <conditionalFormatting sqref="D35">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1314,7 +1429,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
+  <conditionalFormatting sqref="D36">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1325,7 +1440,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
+  <conditionalFormatting sqref="D37">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1336,7 +1451,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="D39">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1347,7 +1462,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
+  <conditionalFormatting sqref="D40">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>

</xml_diff>

<commit_message>
q617 and added leetcode test to q695
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python\leetcode.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA0408E-A5B5-425B-B9CA-C9A04E645EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3C9F1A-4194-440B-82F5-F5E03638ACE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34905" yWindow="3150" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>Problem</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>Max Area of Island</t>
+  </si>
+  <si>
+    <t>Merge Two Binary Trees</t>
   </si>
 </sst>
 </file>
@@ -334,7 +337,28 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="33">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -821,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -936,7 +960,7 @@
       </c>
       <c r="I7" s="10">
         <f ca="1">NOW()</f>
-        <v>44545.580656018516</v>
+        <v>44545.761826041664</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1351,6 +1375,20 @@
       </c>
       <c r="D40" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>617</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="12">
+        <v>44545.755876157411</v>
+      </c>
+      <c r="D41" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1363,7 +1401,18 @@
     <sortCondition descending="1" ref="C2:C12"/>
     <sortCondition descending="1" ref="B2:B12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D30 D38 D41:D101">
+  <conditionalFormatting sqref="D2:D30 D38 D42:D101">
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
     <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1374,7 +1423,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D32">
     <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1385,7 +1434,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D33">
     <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1396,7 +1445,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
+  <conditionalFormatting sqref="D34">
     <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1407,7 +1456,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
+  <conditionalFormatting sqref="D35">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1418,7 +1467,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
+  <conditionalFormatting sqref="D36">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1429,7 +1478,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="D37">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1440,7 +1489,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
+  <conditionalFormatting sqref="D39">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1451,7 +1500,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
+  <conditionalFormatting sqref="D40">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1462,7 +1511,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
+  <conditionalFormatting sqref="D41">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>

</xml_diff>

<commit_message>
q21 and added __bool__() to linked_list.base
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python\leetcode.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B229B2A-A6D2-48B6-9201-25CDB1E62233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A3A656-2573-4545-943E-F798322BB79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="22500" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -919,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="I7" s="10">
         <f ca="1">NOW()</f>
-        <v>44558.894759374998</v>
+        <v>44559.484613541666</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1258,6 +1258,9 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>21</v>
+      </c>
       <c r="B26" s="8" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
q77 and improved qnnn
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python\leetcode.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8244E7-F1AE-4E2C-AEE2-DBD3CEBC5C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F97185-9319-4B6F-85E5-4E0D039019D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>Problem</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>Rotting Oranges</t>
+  </si>
+  <si>
+    <t>Combinations</t>
   </si>
 </sst>
 </file>
@@ -346,7 +349,28 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="45">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -917,20 +941,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="76.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="76.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -947,7 +971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>441</v>
       </c>
@@ -961,7 +985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1489</v>
       </c>
@@ -975,7 +999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>121</v>
       </c>
@@ -992,7 +1016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>122</v>
       </c>
@@ -1009,7 +1033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>35</v>
       </c>
@@ -1020,7 +1044,7 @@
         <v>44516</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>278</v>
       </c>
@@ -1032,10 +1056,10 @@
       </c>
       <c r="I7" s="10">
         <f ca="1">NOW()</f>
-        <v>44559.546144907406</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44564.718163194448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>309</v>
       </c>
@@ -1049,7 +1073,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>704</v>
       </c>
@@ -1060,7 +1084,7 @@
         <v>44516</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>714</v>
       </c>
@@ -1071,7 +1095,7 @@
         <v>44516</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>189</v>
       </c>
@@ -1082,7 +1106,7 @@
         <v>44517</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>977</v>
       </c>
@@ -1093,7 +1117,7 @@
         <v>44517</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>283</v>
       </c>
@@ -1107,7 +1131,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>167</v>
       </c>
@@ -1121,7 +1145,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>344</v>
       </c>
@@ -1135,7 +1159,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>557</v>
       </c>
@@ -1149,7 +1173,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
@@ -1160,7 +1184,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>6</v>
       </c>
@@ -1171,7 +1195,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>11</v>
       </c>
@@ -1182,7 +1206,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
         <v>7</v>
       </c>
@@ -1193,7 +1217,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>328</v>
       </c>
@@ -1207,7 +1231,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>12</v>
       </c>
@@ -1218,7 +1242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>206</v>
       </c>
@@ -1232,7 +1256,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>19</v>
       </c>
@@ -1246,7 +1270,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>234</v>
       </c>
@@ -1260,7 +1284,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>21</v>
       </c>
@@ -1274,7 +1298,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
         <v>16</v>
       </c>
@@ -1285,7 +1309,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1299,7 +1323,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" s="9" t="s">
         <v>40</v>
       </c>
@@ -1307,7 +1331,7 @@
         <v>44536.512189930552</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
         <v>41</v>
       </c>
@@ -1315,7 +1339,7 @@
         <v>44536.543766666669</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>876</v>
       </c>
@@ -1329,7 +1353,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>567</v>
       </c>
@@ -1343,7 +1367,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1357,7 +1381,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>237</v>
       </c>
@@ -1371,7 +1395,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>191</v>
       </c>
@@ -1385,7 +1409,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>973</v>
       </c>
@@ -1399,7 +1423,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>5</v>
       </c>
@@ -1413,7 +1437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1326</v>
       </c>
@@ -1427,7 +1451,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>733</v>
       </c>
@@ -1441,7 +1465,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>695</v>
       </c>
@@ -1455,7 +1479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>617</v>
       </c>
@@ -1469,7 +1493,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>116</v>
       </c>
@@ -1483,7 +1507,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>542</v>
       </c>
@@ -1497,7 +1521,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>994</v>
       </c>
@@ -1508,6 +1532,20 @@
         <v>44558.894684722225</v>
       </c>
       <c r="D44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>77</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="12">
+        <v>44564.717862731479</v>
+      </c>
+      <c r="D45" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1521,7 +1559,18 @@
     <sortCondition descending="1" ref="C2:C12"/>
     <sortCondition descending="1" ref="B2:B12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D30 D38 D45:D101">
+  <conditionalFormatting sqref="D2:D30 D38 D46:D102">
+    <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
     <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1532,7 +1581,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D32">
     <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1543,7 +1592,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D33">
     <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1554,7 +1603,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
+  <conditionalFormatting sqref="D34">
     <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1565,7 +1614,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
+  <conditionalFormatting sqref="D35">
     <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1576,7 +1625,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
+  <conditionalFormatting sqref="D36">
     <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1587,7 +1636,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="D37">
     <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1598,7 +1647,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
+  <conditionalFormatting sqref="D39">
     <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1609,7 +1658,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
+  <conditionalFormatting sqref="D40">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1620,7 +1669,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
+  <conditionalFormatting sqref="D41">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1631,7 +1680,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
+  <conditionalFormatting sqref="D42">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1642,7 +1691,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
+  <conditionalFormatting sqref="D43">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1653,7 +1702,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
+  <conditionalFormatting sqref="D44">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1664,7 +1713,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
+  <conditionalFormatting sqref="D45">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>

</xml_diff>

<commit_message>
q20 and revise qnnn template
revise qnnn template with more common components to save repetitive tasks after cloning qnnn
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python\leetcode.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B824C14A-A2B0-4FA0-BCE6-E45637BCB07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774729F1-4032-481A-8E7A-4DA33BE7BC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
   <si>
     <t>Problem</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>242. Valid Anagram</t>
+  </si>
+  <si>
+    <t>20. Valid Parentheses</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,28 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="105">
+  <dxfs count="108">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1421,10 +1445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1536,7 +1560,7 @@
       </c>
       <c r="I7" s="10">
         <f ca="1">NOW()</f>
-        <v>44574.534476736109</v>
+        <v>44574.618118402781</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2312,6 +2336,20 @@
         <v>44574.529263773147</v>
       </c>
       <c r="D65" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>20</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C66" s="12">
+        <v>44574.617818634259</v>
+      </c>
+      <c r="D66" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2325,7 +2363,18 @@
     <sortCondition descending="1" ref="C2:C12"/>
     <sortCondition descending="1" ref="B2:B12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D30 D38 D66:D102">
+  <conditionalFormatting sqref="D2:D30 D38 D67:D102">
+    <cfRule type="cellIs" dxfId="107" priority="112" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="113" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="114" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
     <cfRule type="cellIs" dxfId="104" priority="109" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2336,7 +2385,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D32">
     <cfRule type="cellIs" dxfId="101" priority="106" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2347,7 +2396,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D33">
     <cfRule type="cellIs" dxfId="98" priority="103" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2358,7 +2407,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
+  <conditionalFormatting sqref="D34">
     <cfRule type="cellIs" dxfId="95" priority="100" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2369,7 +2418,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
+  <conditionalFormatting sqref="D35">
     <cfRule type="cellIs" dxfId="92" priority="97" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2380,7 +2429,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
+  <conditionalFormatting sqref="D36">
     <cfRule type="cellIs" dxfId="89" priority="94" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2391,7 +2440,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="D37">
     <cfRule type="cellIs" dxfId="86" priority="91" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2402,7 +2451,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
+  <conditionalFormatting sqref="D39">
     <cfRule type="cellIs" dxfId="83" priority="88" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2413,7 +2462,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
+  <conditionalFormatting sqref="D40">
     <cfRule type="cellIs" dxfId="80" priority="85" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2424,7 +2473,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
+  <conditionalFormatting sqref="D41">
     <cfRule type="cellIs" dxfId="77" priority="82" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2435,7 +2484,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
+  <conditionalFormatting sqref="D42">
     <cfRule type="cellIs" dxfId="74" priority="79" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2446,7 +2495,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
+  <conditionalFormatting sqref="D43">
     <cfRule type="cellIs" dxfId="71" priority="76" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2457,7 +2506,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
+  <conditionalFormatting sqref="D44">
     <cfRule type="cellIs" dxfId="68" priority="73" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2468,7 +2517,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
+  <conditionalFormatting sqref="D45">
     <cfRule type="cellIs" dxfId="65" priority="70" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2479,7 +2528,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
+  <conditionalFormatting sqref="D46">
     <cfRule type="cellIs" dxfId="62" priority="67" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2490,7 +2539,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
+  <conditionalFormatting sqref="D47">
     <cfRule type="cellIs" dxfId="59" priority="64" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2501,7 +2550,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
+  <conditionalFormatting sqref="D48">
     <cfRule type="cellIs" dxfId="56" priority="61" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2512,7 +2561,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
+  <conditionalFormatting sqref="D49">
     <cfRule type="cellIs" dxfId="53" priority="58" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2523,7 +2572,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
+  <conditionalFormatting sqref="D50">
     <cfRule type="cellIs" dxfId="50" priority="55" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2534,7 +2583,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
+  <conditionalFormatting sqref="D51">
     <cfRule type="cellIs" dxfId="47" priority="52" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2545,7 +2594,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
+  <conditionalFormatting sqref="D52">
     <cfRule type="cellIs" dxfId="44" priority="49" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2556,7 +2605,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
+  <conditionalFormatting sqref="D53">
     <cfRule type="cellIs" dxfId="41" priority="46" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2567,7 +2616,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
+  <conditionalFormatting sqref="D54">
     <cfRule type="cellIs" dxfId="38" priority="43" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2578,7 +2627,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
+  <conditionalFormatting sqref="D55">
     <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2589,7 +2638,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
+  <conditionalFormatting sqref="D56">
     <cfRule type="cellIs" dxfId="32" priority="37" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2600,7 +2649,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
+  <conditionalFormatting sqref="D57">
     <cfRule type="cellIs" dxfId="29" priority="34" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2611,7 +2660,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
+  <conditionalFormatting sqref="D58">
     <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2622,7 +2671,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
+  <conditionalFormatting sqref="D59">
     <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2633,7 +2682,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
+  <conditionalFormatting sqref="D60">
     <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2644,18 +2693,18 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="23" operator="equal">
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D61">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2666,7 +2715,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
+  <conditionalFormatting sqref="D63">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2677,7 +2726,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
+  <conditionalFormatting sqref="D64">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2688,7 +2737,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
+  <conditionalFormatting sqref="D65">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2699,7 +2748,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
+  <conditionalFormatting sqref="D66">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>

</xml_diff>

<commit_message>
q102-binary_tree_04... fix link binary_tree_02,_03
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python\leetcode.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB03781-6E8F-4EB2-BCC3-0B8B8E6BF63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0F12A1-5E23-4C9F-AD94-3565287FDB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-6810" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="83">
   <si>
     <t>Problem</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>binary_tree_03_postorder_traversal</t>
+  </si>
+  <si>
+    <t>binary_tree_04_level_order_traversal</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,28 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="120">
+  <dxfs count="123">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1544,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1659,7 +1683,7 @@
       </c>
       <c r="I7" s="10">
         <f ca="1">NOW()</f>
-        <v>44578.631981250001</v>
+        <v>44578.702202083332</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2520,6 +2544,20 @@
       </c>
       <c r="D71" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>102</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" s="10">
+        <v>44578.702042824072</v>
+      </c>
+      <c r="D72" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2532,7 +2570,18 @@
     <sortCondition descending="1" ref="C2:C12"/>
     <sortCondition descending="1" ref="B2:B12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D30 D38 D69 D72:D102">
+  <conditionalFormatting sqref="D2:D30 D38 D69 D73:D102">
+    <cfRule type="cellIs" dxfId="122" priority="127" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="121" priority="128" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="129" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
     <cfRule type="cellIs" dxfId="119" priority="124" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2543,7 +2592,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D32">
     <cfRule type="cellIs" dxfId="116" priority="121" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2554,7 +2603,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D33">
     <cfRule type="cellIs" dxfId="113" priority="118" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2565,7 +2614,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
+  <conditionalFormatting sqref="D34">
     <cfRule type="cellIs" dxfId="110" priority="115" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2576,7 +2625,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
+  <conditionalFormatting sqref="D35">
     <cfRule type="cellIs" dxfId="107" priority="112" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2587,7 +2636,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
+  <conditionalFormatting sqref="D36">
     <cfRule type="cellIs" dxfId="104" priority="109" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2598,7 +2647,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="D37">
     <cfRule type="cellIs" dxfId="101" priority="106" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2609,7 +2658,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
+  <conditionalFormatting sqref="D39">
     <cfRule type="cellIs" dxfId="98" priority="103" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2620,7 +2669,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
+  <conditionalFormatting sqref="D40">
     <cfRule type="cellIs" dxfId="95" priority="100" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2631,7 +2680,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
+  <conditionalFormatting sqref="D41">
     <cfRule type="cellIs" dxfId="92" priority="97" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2642,7 +2691,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
+  <conditionalFormatting sqref="D42">
     <cfRule type="cellIs" dxfId="89" priority="94" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2653,7 +2702,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
+  <conditionalFormatting sqref="D43">
     <cfRule type="cellIs" dxfId="86" priority="91" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2664,7 +2713,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
+  <conditionalFormatting sqref="D44">
     <cfRule type="cellIs" dxfId="83" priority="88" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2675,7 +2724,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
+  <conditionalFormatting sqref="D45">
     <cfRule type="cellIs" dxfId="80" priority="85" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2686,7 +2735,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
+  <conditionalFormatting sqref="D46">
     <cfRule type="cellIs" dxfId="77" priority="82" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2697,7 +2746,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
+  <conditionalFormatting sqref="D47">
     <cfRule type="cellIs" dxfId="74" priority="79" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2708,7 +2757,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
+  <conditionalFormatting sqref="D48">
     <cfRule type="cellIs" dxfId="71" priority="76" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2719,7 +2768,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
+  <conditionalFormatting sqref="D49">
     <cfRule type="cellIs" dxfId="68" priority="73" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2730,7 +2779,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
+  <conditionalFormatting sqref="D50">
     <cfRule type="cellIs" dxfId="65" priority="70" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2741,7 +2790,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
+  <conditionalFormatting sqref="D51">
     <cfRule type="cellIs" dxfId="62" priority="67" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2752,7 +2801,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
+  <conditionalFormatting sqref="D52">
     <cfRule type="cellIs" dxfId="59" priority="64" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2763,7 +2812,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
+  <conditionalFormatting sqref="D53">
     <cfRule type="cellIs" dxfId="56" priority="61" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2774,7 +2823,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
+  <conditionalFormatting sqref="D54">
     <cfRule type="cellIs" dxfId="53" priority="58" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2785,7 +2834,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
+  <conditionalFormatting sqref="D55">
     <cfRule type="cellIs" dxfId="50" priority="55" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2796,7 +2845,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
+  <conditionalFormatting sqref="D56">
     <cfRule type="cellIs" dxfId="47" priority="52" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2807,7 +2856,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
+  <conditionalFormatting sqref="D57">
     <cfRule type="cellIs" dxfId="44" priority="49" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2818,7 +2867,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
+  <conditionalFormatting sqref="D58">
     <cfRule type="cellIs" dxfId="41" priority="46" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2829,7 +2878,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
+  <conditionalFormatting sqref="D59">
     <cfRule type="cellIs" dxfId="38" priority="43" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2840,7 +2889,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
+  <conditionalFormatting sqref="D60">
     <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2851,18 +2900,18 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="cellIs" dxfId="32" priority="37" operator="equal">
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="38" operator="equal">
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D61">
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
     <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2873,7 +2922,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
+  <conditionalFormatting sqref="D63">
     <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2884,7 +2933,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
+  <conditionalFormatting sqref="D64">
     <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2895,7 +2944,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
+  <conditionalFormatting sqref="D65">
     <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2906,7 +2955,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
+  <conditionalFormatting sqref="D66">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2917,7 +2966,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
+  <conditionalFormatting sqref="D67">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2928,7 +2977,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
+  <conditionalFormatting sqref="D68">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2939,7 +2988,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
+  <conditionalFormatting sqref="D70">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2950,7 +2999,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D70">
+  <conditionalFormatting sqref="D71">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2961,7 +3010,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D71">
+  <conditionalFormatting sqref="D72">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>

</xml_diff>

<commit_message>
q112 - binary_tree_07_path_sum, fix qnnn
qnnn fixed to pass pytest.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python\leetcode.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C34078-42BC-48A9-87E2-AE5E9D818FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E0B4DC-A032-41FA-9623-5B584E6A21A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30510" yWindow="720" windowWidth="12150" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43455" yWindow="780" windowWidth="12150" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="86">
   <si>
     <t>Problem</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>binary_tree_06_symmetric_tree</t>
+  </si>
+  <si>
+    <t>binary_tree_07_path_sum</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,28 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="129">
+  <dxfs count="132">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1616,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1731,7 +1755,7 @@
       </c>
       <c r="I7" s="10">
         <f ca="1">NOW()</f>
-        <v>44579.67350300926</v>
+        <v>44579.69975</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2633,6 +2657,20 @@
         <v>44579.673372106481</v>
       </c>
       <c r="D74" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>112</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75" s="10">
+        <v>44579.699618055558</v>
+      </c>
+      <c r="D75" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2646,7 +2684,18 @@
     <sortCondition descending="1" ref="C2:C12"/>
     <sortCondition descending="1" ref="B2:B12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D30 D38 D69 D75:D102">
+  <conditionalFormatting sqref="D2:D30 D38 D69 D76:D102">
+    <cfRule type="cellIs" dxfId="131" priority="136" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="137" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="129" priority="138" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
     <cfRule type="cellIs" dxfId="128" priority="133" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2657,7 +2706,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D32">
     <cfRule type="cellIs" dxfId="125" priority="130" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2668,7 +2717,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D33">
     <cfRule type="cellIs" dxfId="122" priority="127" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2679,7 +2728,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
+  <conditionalFormatting sqref="D34">
     <cfRule type="cellIs" dxfId="119" priority="124" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2690,7 +2739,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
+  <conditionalFormatting sqref="D35">
     <cfRule type="cellIs" dxfId="116" priority="121" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2701,7 +2750,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
+  <conditionalFormatting sqref="D36">
     <cfRule type="cellIs" dxfId="113" priority="118" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2712,7 +2761,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="D37">
     <cfRule type="cellIs" dxfId="110" priority="115" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2723,7 +2772,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
+  <conditionalFormatting sqref="D39">
     <cfRule type="cellIs" dxfId="107" priority="112" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2734,7 +2783,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
+  <conditionalFormatting sqref="D40">
     <cfRule type="cellIs" dxfId="104" priority="109" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2745,7 +2794,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
+  <conditionalFormatting sqref="D41">
     <cfRule type="cellIs" dxfId="101" priority="106" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2756,7 +2805,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
+  <conditionalFormatting sqref="D42">
     <cfRule type="cellIs" dxfId="98" priority="103" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2767,7 +2816,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
+  <conditionalFormatting sqref="D43">
     <cfRule type="cellIs" dxfId="95" priority="100" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2778,7 +2827,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
+  <conditionalFormatting sqref="D44">
     <cfRule type="cellIs" dxfId="92" priority="97" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2789,7 +2838,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
+  <conditionalFormatting sqref="D45">
     <cfRule type="cellIs" dxfId="89" priority="94" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2800,7 +2849,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
+  <conditionalFormatting sqref="D46">
     <cfRule type="cellIs" dxfId="86" priority="91" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2811,7 +2860,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
+  <conditionalFormatting sqref="D47">
     <cfRule type="cellIs" dxfId="83" priority="88" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2822,7 +2871,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
+  <conditionalFormatting sqref="D48">
     <cfRule type="cellIs" dxfId="80" priority="85" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2833,7 +2882,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
+  <conditionalFormatting sqref="D49">
     <cfRule type="cellIs" dxfId="77" priority="82" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2844,7 +2893,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
+  <conditionalFormatting sqref="D50">
     <cfRule type="cellIs" dxfId="74" priority="79" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2855,7 +2904,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
+  <conditionalFormatting sqref="D51">
     <cfRule type="cellIs" dxfId="71" priority="76" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2866,7 +2915,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
+  <conditionalFormatting sqref="D52">
     <cfRule type="cellIs" dxfId="68" priority="73" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2877,7 +2926,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
+  <conditionalFormatting sqref="D53">
     <cfRule type="cellIs" dxfId="65" priority="70" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2888,7 +2937,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
+  <conditionalFormatting sqref="D54">
     <cfRule type="cellIs" dxfId="62" priority="67" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2899,7 +2948,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
+  <conditionalFormatting sqref="D55">
     <cfRule type="cellIs" dxfId="59" priority="64" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2910,7 +2959,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
+  <conditionalFormatting sqref="D56">
     <cfRule type="cellIs" dxfId="56" priority="61" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2921,7 +2970,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
+  <conditionalFormatting sqref="D57">
     <cfRule type="cellIs" dxfId="53" priority="58" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2932,7 +2981,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
+  <conditionalFormatting sqref="D58">
     <cfRule type="cellIs" dxfId="50" priority="55" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2943,7 +2992,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
+  <conditionalFormatting sqref="D59">
     <cfRule type="cellIs" dxfId="47" priority="52" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2954,7 +3003,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
+  <conditionalFormatting sqref="D60">
     <cfRule type="cellIs" dxfId="44" priority="49" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2965,18 +3014,18 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="cellIs" dxfId="41" priority="46" operator="equal">
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="47" operator="equal">
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="48" operator="equal">
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D61">
+    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="42" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
     <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2987,7 +3036,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
+  <conditionalFormatting sqref="D63">
     <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2998,7 +3047,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
+  <conditionalFormatting sqref="D64">
     <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3009,7 +3058,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
+  <conditionalFormatting sqref="D65">
     <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3020,7 +3069,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
+  <conditionalFormatting sqref="D66">
     <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3031,7 +3080,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
+  <conditionalFormatting sqref="D67">
     <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3042,7 +3091,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
+  <conditionalFormatting sqref="D68">
     <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3053,7 +3102,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
+  <conditionalFormatting sqref="D70">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3064,7 +3113,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D70">
+  <conditionalFormatting sqref="D71">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3075,7 +3124,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D71">
+  <conditionalFormatting sqref="D72">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3086,7 +3135,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D72">
+  <conditionalFormatting sqref="D73">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3097,7 +3146,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D73">
+  <conditionalFormatting sqref="D74">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3108,7 +3157,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D74">
+  <conditionalFormatting sqref="D75">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>

</xml_diff>

<commit_message>
q700 and revised q226
Finished q700
Added question link to q226
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python\leetcode.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DFD6C5-3336-470E-8FC0-C8B80A6D7546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176EB372-8123-42FE-AA10-78EC64E843BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43455" yWindow="780" windowWidth="12150" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="88">
   <si>
     <t>Problem</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t>226. Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>700. Search in a Binary Search Tree</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,28 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="135">
+  <dxfs count="138">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1664,20 +1688,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="76.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="76.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1694,7 +1718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>441</v>
       </c>
@@ -1708,7 +1732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1489</v>
       </c>
@@ -1722,7 +1746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>122</v>
       </c>
@@ -1739,7 +1763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>35</v>
       </c>
@@ -1753,7 +1777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>278</v>
       </c>
@@ -1764,7 +1788,7 @@
         <v>44516</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>309</v>
       </c>
@@ -1779,10 +1803,10 @@
       </c>
       <c r="I7" s="10">
         <f ca="1">NOW()</f>
-        <v>44579.721841550927</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44580.481789467594</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>704</v>
       </c>
@@ -1793,7 +1817,7 @@
         <v>44516</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>714</v>
       </c>
@@ -1804,7 +1828,7 @@
         <v>44516</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>189</v>
       </c>
@@ -1815,7 +1839,7 @@
         <v>44517</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>977</v>
       </c>
@@ -1826,7 +1850,7 @@
         <v>44517</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>283</v>
       </c>
@@ -1840,7 +1864,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>167</v>
       </c>
@@ -1854,7 +1878,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>344</v>
       </c>
@@ -1868,7 +1892,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>557</v>
       </c>
@@ -1882,7 +1906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
@@ -1893,7 +1917,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
@@ -1904,7 +1928,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>141</v>
       </c>
@@ -1918,7 +1942,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>7</v>
       </c>
@@ -1929,7 +1953,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>328</v>
       </c>
@@ -1943,7 +1967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>203</v>
       </c>
@@ -1957,7 +1981,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>206</v>
       </c>
@@ -1971,7 +1995,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1985,7 +2009,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>234</v>
       </c>
@@ -1999,7 +2023,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -2013,7 +2037,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>16</v>
       </c>
@@ -2024,7 +2048,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -2038,7 +2062,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
         <v>40</v>
       </c>
@@ -2046,7 +2070,7 @@
         <v>44536.512189930552</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>41</v>
       </c>
@@ -2054,7 +2078,7 @@
         <v>44536.543766666669</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>876</v>
       </c>
@@ -2068,7 +2092,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>567</v>
       </c>
@@ -2082,7 +2106,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2096,7 +2120,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>237</v>
       </c>
@@ -2110,7 +2134,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>191</v>
       </c>
@@ -2124,7 +2148,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>973</v>
       </c>
@@ -2138,7 +2162,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -2152,7 +2176,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1326</v>
       </c>
@@ -2166,7 +2190,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>733</v>
       </c>
@@ -2180,7 +2204,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>695</v>
       </c>
@@ -2194,7 +2218,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>617</v>
       </c>
@@ -2208,7 +2232,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>116</v>
       </c>
@@ -2222,7 +2246,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>542</v>
       </c>
@@ -2236,7 +2260,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>994</v>
       </c>
@@ -2250,7 +2274,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>77</v>
       </c>
@@ -2264,7 +2288,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>46</v>
       </c>
@@ -2278,7 +2302,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>781</v>
       </c>
@@ -2292,7 +2316,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>70</v>
       </c>
@@ -2306,7 +2330,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>198</v>
       </c>
@@ -2320,7 +2344,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>120</v>
       </c>
@@ -2334,7 +2358,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>231</v>
       </c>
@@ -2348,7 +2372,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>190</v>
       </c>
@@ -2362,7 +2386,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>136</v>
       </c>
@@ -2376,7 +2400,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>217</v>
       </c>
@@ -2390,7 +2414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2404,7 +2428,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1</v>
       </c>
@@ -2418,7 +2442,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>88</v>
       </c>
@@ -2432,7 +2456,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>350</v>
       </c>
@@ -2446,7 +2470,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>121</v>
       </c>
@@ -2460,7 +2484,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>566</v>
       </c>
@@ -2474,7 +2498,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>118</v>
       </c>
@@ -2488,7 +2512,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>36</v>
       </c>
@@ -2502,7 +2526,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>74</v>
       </c>
@@ -2516,7 +2540,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>387</v>
       </c>
@@ -2530,7 +2554,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>383</v>
       </c>
@@ -2544,7 +2568,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>242</v>
       </c>
@@ -2558,7 +2582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>20</v>
       </c>
@@ -2572,7 +2596,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>232</v>
       </c>
@@ -2586,7 +2610,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>83</v>
       </c>
@@ -2600,7 +2624,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>144</v>
       </c>
@@ -2614,7 +2638,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>94</v>
       </c>
@@ -2628,7 +2652,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>145</v>
       </c>
@@ -2642,7 +2666,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>102</v>
       </c>
@@ -2656,7 +2680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>104</v>
       </c>
@@ -2670,7 +2694,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>101</v>
       </c>
@@ -2684,7 +2708,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>112</v>
       </c>
@@ -2698,7 +2722,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>226</v>
       </c>
@@ -2709,6 +2733,20 @@
         <v>44579.721729282406</v>
       </c>
       <c r="D76" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>700</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C77" s="10">
+        <v>44579.746840277781</v>
+      </c>
+      <c r="D77" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2722,7 +2760,18 @@
     <sortCondition descending="1" ref="C2:C12"/>
     <sortCondition descending="1" ref="B2:B12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D30 D38 D69 D77:D102">
+  <conditionalFormatting sqref="D2:D30 D38 D69 D78:D102">
+    <cfRule type="cellIs" dxfId="137" priority="142" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="136" priority="143" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="135" priority="144" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
     <cfRule type="cellIs" dxfId="134" priority="139" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2733,7 +2782,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D32">
     <cfRule type="cellIs" dxfId="131" priority="136" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2744,7 +2793,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D33">
     <cfRule type="cellIs" dxfId="128" priority="133" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2755,7 +2804,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
+  <conditionalFormatting sqref="D34">
     <cfRule type="cellIs" dxfId="125" priority="130" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2766,7 +2815,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
+  <conditionalFormatting sqref="D35">
     <cfRule type="cellIs" dxfId="122" priority="127" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2777,7 +2826,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
+  <conditionalFormatting sqref="D36">
     <cfRule type="cellIs" dxfId="119" priority="124" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2788,7 +2837,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="D37">
     <cfRule type="cellIs" dxfId="116" priority="121" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2799,7 +2848,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
+  <conditionalFormatting sqref="D39">
     <cfRule type="cellIs" dxfId="113" priority="118" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2810,7 +2859,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
+  <conditionalFormatting sqref="D40">
     <cfRule type="cellIs" dxfId="110" priority="115" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2821,7 +2870,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
+  <conditionalFormatting sqref="D41">
     <cfRule type="cellIs" dxfId="107" priority="112" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2832,7 +2881,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
+  <conditionalFormatting sqref="D42">
     <cfRule type="cellIs" dxfId="104" priority="109" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2843,7 +2892,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
+  <conditionalFormatting sqref="D43">
     <cfRule type="cellIs" dxfId="101" priority="106" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2854,7 +2903,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
+  <conditionalFormatting sqref="D44">
     <cfRule type="cellIs" dxfId="98" priority="103" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2865,7 +2914,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
+  <conditionalFormatting sqref="D45">
     <cfRule type="cellIs" dxfId="95" priority="100" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2876,7 +2925,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
+  <conditionalFormatting sqref="D46">
     <cfRule type="cellIs" dxfId="92" priority="97" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2887,7 +2936,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
+  <conditionalFormatting sqref="D47">
     <cfRule type="cellIs" dxfId="89" priority="94" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2898,7 +2947,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
+  <conditionalFormatting sqref="D48">
     <cfRule type="cellIs" dxfId="86" priority="91" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2909,7 +2958,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
+  <conditionalFormatting sqref="D49">
     <cfRule type="cellIs" dxfId="83" priority="88" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2920,7 +2969,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
+  <conditionalFormatting sqref="D50">
     <cfRule type="cellIs" dxfId="80" priority="85" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2931,7 +2980,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
+  <conditionalFormatting sqref="D51">
     <cfRule type="cellIs" dxfId="77" priority="82" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2942,7 +2991,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
+  <conditionalFormatting sqref="D52">
     <cfRule type="cellIs" dxfId="74" priority="79" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2953,7 +3002,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
+  <conditionalFormatting sqref="D53">
     <cfRule type="cellIs" dxfId="71" priority="76" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2964,7 +3013,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
+  <conditionalFormatting sqref="D54">
     <cfRule type="cellIs" dxfId="68" priority="73" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2975,7 +3024,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
+  <conditionalFormatting sqref="D55">
     <cfRule type="cellIs" dxfId="65" priority="70" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2986,7 +3035,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
+  <conditionalFormatting sqref="D56">
     <cfRule type="cellIs" dxfId="62" priority="67" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2997,7 +3046,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
+  <conditionalFormatting sqref="D57">
     <cfRule type="cellIs" dxfId="59" priority="64" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3008,7 +3057,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
+  <conditionalFormatting sqref="D58">
     <cfRule type="cellIs" dxfId="56" priority="61" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3019,7 +3068,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
+  <conditionalFormatting sqref="D59">
     <cfRule type="cellIs" dxfId="53" priority="58" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3030,7 +3079,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
+  <conditionalFormatting sqref="D60">
     <cfRule type="cellIs" dxfId="50" priority="55" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3041,18 +3090,18 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="cellIs" dxfId="47" priority="52" operator="equal">
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="53" operator="equal">
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D61">
+    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
     <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3063,7 +3112,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
+  <conditionalFormatting sqref="D63">
     <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3074,7 +3123,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
+  <conditionalFormatting sqref="D64">
     <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3085,7 +3134,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
+  <conditionalFormatting sqref="D65">
     <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3096,7 +3145,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
+  <conditionalFormatting sqref="D66">
     <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3107,7 +3156,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
+  <conditionalFormatting sqref="D67">
     <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3118,7 +3167,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
+  <conditionalFormatting sqref="D68">
     <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3129,7 +3178,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
+  <conditionalFormatting sqref="D70">
     <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3140,7 +3189,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D70">
+  <conditionalFormatting sqref="D71">
     <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3151,7 +3200,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D71">
+  <conditionalFormatting sqref="D72">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3162,7 +3211,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D72">
+  <conditionalFormatting sqref="D73">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3173,7 +3222,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D73">
+  <conditionalFormatting sqref="D74">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3184,7 +3233,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D74">
+  <conditionalFormatting sqref="D75">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3195,7 +3244,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D75">
+  <conditionalFormatting sqref="D76">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -3206,7 +3255,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D76">
+  <conditionalFormatting sqref="D77">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>

</xml_diff>